<commit_message>
updating UH002 + ABR plots
</commit_message>
<xml_diff>
--- a/sub_info.xlsx
+++ b/sub_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="128">
   <si>
     <t xml:space="preserve">UHEAL ID</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">UH002</t>
   </si>
   <si>
+    <t xml:space="preserve">PHY1</t>
+  </si>
+  <si>
     <t xml:space="preserve">UH003</t>
   </si>
   <si>
@@ -133,6 +136,9 @@
     <t xml:space="preserve">UH030</t>
   </si>
   <si>
+    <t xml:space="preserve">UH031</t>
+  </si>
+  <si>
     <t xml:space="preserve">Y </t>
   </si>
   <si>
@@ -323,9 +329,6 @@
   </si>
   <si>
     <t xml:space="preserve">UH092</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHY1</t>
   </si>
   <si>
     <t xml:space="preserve">UH093</t>
@@ -525,8 +528,8 @@
   </sheetPr>
   <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D122" activeCellId="0" sqref="D122"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -571,7 +574,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -582,7 +585,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>5</v>
@@ -593,7 +596,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>5</v>
@@ -604,7 +607,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>5</v>
@@ -615,7 +618,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>5</v>
@@ -629,7 +632,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>5</v>
@@ -640,7 +643,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>5</v>
@@ -654,7 +657,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>5</v>
@@ -665,7 +668,7 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>5</v>
@@ -679,7 +682,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>5</v>
@@ -693,7 +696,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>5</v>
@@ -707,7 +710,7 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>5</v>
@@ -721,13 +724,13 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>7</v>
@@ -735,7 +738,7 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>5</v>
@@ -749,7 +752,7 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>5</v>
@@ -763,7 +766,7 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>5</v>
@@ -774,7 +777,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>5</v>
@@ -785,7 +788,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>5</v>
@@ -799,7 +802,7 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>5</v>
@@ -813,7 +816,7 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>5</v>
@@ -824,7 +827,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>5</v>
@@ -838,13 +841,13 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>7</v>
@@ -852,13 +855,13 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>7</v>
@@ -866,7 +869,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>5</v>
@@ -880,7 +883,7 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>5</v>
@@ -891,7 +894,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>5</v>
@@ -905,7 +908,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>5</v>
@@ -916,7 +919,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>5</v>
@@ -926,17 +929,22 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="B31" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="D31" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>5</v>
@@ -950,7 +958,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>5</v>
@@ -964,7 +972,7 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>5</v>
@@ -978,7 +986,7 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>5</v>
@@ -992,7 +1000,7 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>5</v>
@@ -1006,7 +1014,7 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>5</v>
@@ -1020,7 +1028,7 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>5</v>
@@ -1031,7 +1039,7 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>5</v>
@@ -1045,7 +1053,7 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>5</v>
@@ -1059,7 +1067,7 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>5</v>
@@ -1073,13 +1081,13 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>7</v>
@@ -1087,7 +1095,7 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>5</v>
@@ -1098,7 +1106,7 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>5</v>
@@ -1109,24 +1117,24 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>7</v>
@@ -1134,7 +1142,7 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>5</v>
@@ -1145,7 +1153,7 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>5</v>
@@ -1159,7 +1167,7 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>5</v>
@@ -1173,7 +1181,7 @@
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>5</v>
@@ -1184,7 +1192,7 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>5</v>
@@ -1195,7 +1203,7 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>5</v>
@@ -1209,7 +1217,7 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>5</v>
@@ -1223,7 +1231,7 @@
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>5</v>
@@ -1234,7 +1242,7 @@
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>5</v>
@@ -1245,7 +1253,7 @@
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>5</v>
@@ -1259,7 +1267,7 @@
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>5</v>
@@ -1273,7 +1281,7 @@
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>5</v>
@@ -1287,7 +1295,7 @@
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>5</v>
@@ -1298,7 +1306,7 @@
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>5</v>
@@ -1312,7 +1320,7 @@
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>5</v>
@@ -1323,7 +1331,7 @@
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>5</v>
@@ -1334,18 +1342,18 @@
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>5</v>
@@ -1359,7 +1367,7 @@
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>5</v>
@@ -1370,7 +1378,7 @@
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>5</v>
@@ -1384,7 +1392,7 @@
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>5</v>
@@ -1398,7 +1406,7 @@
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>5</v>
@@ -1412,7 +1420,7 @@
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>5</v>
@@ -1426,7 +1434,7 @@
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>5</v>
@@ -1440,7 +1448,7 @@
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>5</v>
@@ -1454,7 +1462,7 @@
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>5</v>
@@ -1465,7 +1473,7 @@
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>5</v>
@@ -1479,7 +1487,7 @@
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>5</v>
@@ -1490,7 +1498,7 @@
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>5</v>
@@ -1501,7 +1509,7 @@
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>5</v>
@@ -1515,7 +1523,7 @@
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>5</v>
@@ -1526,7 +1534,7 @@
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>5</v>
@@ -1537,13 +1545,13 @@
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D79" s="0" t="s">
         <v>7</v>
@@ -1551,7 +1559,7 @@
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>5</v>
@@ -1562,7 +1570,7 @@
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>5</v>
@@ -1573,7 +1581,7 @@
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>5</v>
@@ -1584,7 +1592,7 @@
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>5</v>
@@ -1598,21 +1606,21 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>5</v>
@@ -1621,12 +1629,12 @@
         <v>6</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>5</v>
@@ -1635,12 +1643,12 @@
         <v>6</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>5</v>
@@ -1649,12 +1657,12 @@
         <v>6</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>5</v>
@@ -1663,12 +1671,12 @@
         <v>6</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>5</v>
@@ -1677,399 +1685,399 @@
         <v>6</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C113" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C114" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C116" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>